<commit_message>
updated LIV reference point for wages to average wage. need to re-examine the LIV trend and adjust to reflect changes in wages to average wages per year
</commit_message>
<xml_diff>
--- a/region2017/reports/documents/goal_description_table.xlsx
+++ b/region2017/reports/documents/goal_description_table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="3060" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -648,7 +648,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,7 +730,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="8"/>

</xml_diff>